<commit_message>
updated the default protocol sheets to use jxls3
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/protocol/Protocol-A4.xlsx
+++ b/owlcms/src/main/resources/templates/protocol/Protocol-A4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C658126-391C-4FC7-98D4-EE699835444A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37139799-5879-4FE3-AAED-5E462455C8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="705" windowWidth="23985" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="2235" windowWidth="23985" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="athletes" var="group" groupBy="group.displayCategory" groupOrder="ASC" lastCell="V10")</t>
+          <t>jx:each(items="athletes" var="group" groupBy="group.categorySortCode" groupOrder="ASC" lastCell="V10")</t>
         </r>
       </text>
     </comment>
@@ -1284,10 +1284,46 @@
     <xf numFmtId="0" fontId="31" fillId="13" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1306,42 +1342,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1866,20 +1866,20 @@
       <c r="J1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="115" t="s">
+      <c r="K1" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="108"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="108"/>
+      <c r="P1" s="108"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
     </row>
     <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="54" t="s">
@@ -1916,13 +1916,13 @@
       <c r="J3" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="112" t="s">
+      <c r="K3" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
+      <c r="O3" s="122"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="62"/>
       <c r="R3" s="33" t="s">
@@ -1964,32 +1964,32 @@
       <c r="H6" s="7"/>
       <c r="I6" s="9"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="108" t="s">
+      <c r="K6" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="123"/>
-      <c r="M6" s="109"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="119"/>
       <c r="N6" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="O6" s="108" t="s">
+      <c r="O6" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="123"/>
-      <c r="Q6" s="109"/>
+      <c r="P6" s="118"/>
+      <c r="Q6" s="119"/>
       <c r="R6" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="S6" s="120" t="s">
+      <c r="S6" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="T6" s="118" t="s">
+      <c r="T6" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="116" t="s">
+      <c r="U6" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="V6" s="116" t="s">
+      <c r="V6" s="110" t="s">
         <v>93</v>
       </c>
       <c r="X6"/>
@@ -2007,10 +2007,10 @@
       <c r="D7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="109"/>
+      <c r="F7" s="119"/>
       <c r="G7" s="11" t="s">
         <v>39</v>
       </c>
@@ -2047,10 +2047,10 @@
       <c r="R7" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="S7" s="121"/>
-      <c r="T7" s="119"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
+      <c r="S7" s="115"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="111"/>
+      <c r="V7" s="111"/>
     </row>
     <row r="8" spans="1:24" s="28" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="69"/>
@@ -2106,10 +2106,10 @@
       <c r="D10" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="E10" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="111"/>
+      <c r="F10" s="121"/>
       <c r="G10" s="67" t="s">
         <v>5</v>
       </c>
@@ -2306,23 +2306,23 @@
       <c r="A16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="E16" s="113" t="s">
+      <c r="E16" s="123" t="s">
         <v>53</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="15"/>
       <c r="I16" s="14"/>
-      <c r="J16" s="114" t="s">
+      <c r="J16" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="114"/>
+      <c r="K16" s="109"/>
       <c r="L16" s="14"/>
       <c r="N16" s="16"/>
       <c r="P16" s="14"/>
-      <c r="Q16" s="122" t="s">
+      <c r="Q16" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="R16" s="122"/>
+      <c r="R16" s="116"/>
       <c r="S16" s="48"/>
       <c r="T16" s="14"/>
       <c r="U16" s="12"/>
@@ -2341,15 +2341,15 @@
         <v>27</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="113"/>
+      <c r="E17" s="123"/>
       <c r="F17" s="42" t="s">
         <v>76</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="114"/>
-      <c r="K17" s="114"/>
+      <c r="J17" s="109"/>
+      <c r="K17" s="109"/>
       <c r="L17" s="42" t="s">
         <v>23</v>
       </c>
@@ -2357,8 +2357,8 @@
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="19"/>
-      <c r="Q17" s="122"/>
-      <c r="R17" s="122"/>
+      <c r="Q17" s="116"/>
+      <c r="R17" s="116"/>
       <c r="S17" s="42" t="s">
         <v>87</v>
       </c>
@@ -2396,10 +2396,10 @@
       <c r="E19" s="31"/>
       <c r="F19" s="14"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="114" t="s">
+      <c r="J19" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="K19" s="114"/>
+      <c r="K19" s="109"/>
       <c r="M19"/>
       <c r="N19" s="1"/>
       <c r="O19" s="12"/>
@@ -2427,8 +2427,8 @@
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="114"/>
-      <c r="K20" s="114"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
       <c r="L20" s="42" t="s">
         <v>26</v>
       </c>
@@ -2851,6 +2851,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="14">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="J16:K17"/>
     <mergeCell ref="K1:V1"/>
     <mergeCell ref="J19:K20"/>
     <mergeCell ref="U6:U7"/>
@@ -2860,11 +2865,6 @@
     <mergeCell ref="Q16:R17"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="J16:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:D8">
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">

</xml_diff>